<commit_message>
feat: unical ids of dialog
</commit_message>
<xml_diff>
--- a/[source]/generate/_generator/02_set_includes.xlsx
+++ b/[source]/generate/_generator/02_set_includes.xlsx
@@ -492,7 +492,11 @@
           <t>test</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>test.</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr">
         <is>
           <t>test</t>
@@ -514,7 +518,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>['quest67', 'test.hero', 'test.npc', 'test.remarka']</t>
+          <t>['test.quest67', 'test.test.hero', 'test.test.npc', 'test.test.remarka']</t>
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
@@ -542,7 +546,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>quest67</t>
+          <t>test.quest67</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -559,7 +563,7 @@
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
-          <t>['answer66', 'answer19', 'answer4']</t>
+          <t>['test.answer66', 'test.answer19', 'test.answer4']</t>
         </is>
       </c>
       <c r="I3" t="inlineStr"/>
@@ -581,12 +585,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>answer66</t>
+          <t>test.answer66</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>quest67</t>
+          <t>test.quest67</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -598,7 +602,7 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>['quest65']</t>
+          <t>['test.quest65']</t>
         </is>
       </c>
       <c r="I4" t="inlineStr"/>
@@ -619,12 +623,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>answer19</t>
+          <t>test.answer19</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>quest67</t>
+          <t>test.quest67</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -636,7 +640,7 @@
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
-          <t>['quest18']</t>
+          <t>['test.quest18']</t>
         </is>
       </c>
       <c r="I5" t="inlineStr"/>
@@ -655,12 +659,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>answer4</t>
+          <t>test.answer4</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>quest67</t>
+          <t>test.quest67</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -672,7 +676,7 @@
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
-          <t>['quest3', 'quest1']</t>
+          <t>['test.quest3', 'test.quest1']</t>
         </is>
       </c>
       <c r="I6" t="inlineStr"/>
@@ -696,12 +700,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>quest3</t>
+          <t>test.quest3</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>answer4</t>
+          <t>test.answer4</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -713,7 +717,7 @@
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
-          <t>['answer2']</t>
+          <t>['test.answer2']</t>
         </is>
       </c>
       <c r="I7" t="inlineStr"/>
@@ -738,12 +742,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>quest1</t>
+          <t>test.quest1</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>answer4</t>
+          <t>test.answer4</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -773,12 +777,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>answer2</t>
+          <t>test.answer2</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>quest3</t>
+          <t>test.quest3</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -809,12 +813,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>quest18</t>
+          <t>test.quest18</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>answer19</t>
+          <t>test.answer19</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -826,7 +830,7 @@
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
-          <t>['answer17', 'answer14', 'answer10']</t>
+          <t>['test.answer17', 'test.answer14', 'test.answer10']</t>
         </is>
       </c>
       <c r="I10" t="inlineStr"/>
@@ -847,12 +851,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>answer17</t>
+          <t>test.answer17</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>quest18</t>
+          <t>test.quest18</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -864,7 +868,7 @@
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
-          <t>['quest16']</t>
+          <t>['test.quest16']</t>
         </is>
       </c>
       <c r="I11" t="inlineStr"/>
@@ -892,12 +896,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>answer14</t>
+          <t>test.answer14</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>quest18</t>
+          <t>test.quest18</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -909,7 +913,7 @@
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
         <is>
-          <t>['quest13']</t>
+          <t>['test.quest13']</t>
         </is>
       </c>
       <c r="I12" t="inlineStr"/>
@@ -930,12 +934,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>answer10</t>
+          <t>test.answer10</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>quest18</t>
+          <t>test.quest18</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -947,7 +951,7 @@
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
-          <t>['quest9']</t>
+          <t>['test.quest9']</t>
         </is>
       </c>
       <c r="I13" t="inlineStr"/>
@@ -967,12 +971,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>quest9</t>
+          <t>test.quest9</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>answer10</t>
+          <t>test.answer10</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -984,7 +988,7 @@
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
-          <t>['answer8', 'answer7']</t>
+          <t>['test.answer8', 'test.answer7']</t>
         </is>
       </c>
       <c r="I14" t="inlineStr"/>
@@ -1005,12 +1009,12 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>answer8</t>
+          <t>test.answer8</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>quest9</t>
+          <t>test.quest9</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -1044,12 +1048,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>answer7</t>
+          <t>test.answer7</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>quest9</t>
+          <t>test.quest9</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -1061,7 +1065,7 @@
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr">
         <is>
-          <t>['quest6']</t>
+          <t>['test.quest6']</t>
         </is>
       </c>
       <c r="I16" t="inlineStr"/>
@@ -1086,12 +1090,12 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>quest6</t>
+          <t>test.quest6</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>answer7</t>
+          <t>test.answer7</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
@@ -1103,7 +1107,7 @@
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr">
         <is>
-          <t>['answer5']</t>
+          <t>['test.answer5']</t>
         </is>
       </c>
       <c r="I17" t="inlineStr"/>
@@ -1121,12 +1125,12 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>answer5</t>
+          <t>test.answer5</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>quest6</t>
+          <t>test.quest6</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -1157,12 +1161,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>quest13</t>
+          <t>test.quest13</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>answer14</t>
+          <t>test.answer14</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -1174,7 +1178,7 @@
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
-          <t>['answer12', 'answer11']</t>
+          <t>['test.answer12', 'test.answer11']</t>
         </is>
       </c>
       <c r="I19" t="inlineStr"/>
@@ -1195,12 +1199,12 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>answer12</t>
+          <t>test.answer12</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>quest13</t>
+          <t>test.quest13</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -1232,12 +1236,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>answer11</t>
+          <t>test.answer11</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>quest13</t>
+          <t>test.quest13</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
@@ -1268,12 +1272,12 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>quest16</t>
+          <t>test.quest16</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>answer17</t>
+          <t>test.answer17</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
@@ -1285,7 +1289,7 @@
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr">
         <is>
-          <t>['answer15']</t>
+          <t>['test.answer15']</t>
         </is>
       </c>
       <c r="I22" t="inlineStr"/>
@@ -1306,12 +1310,12 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>answer15</t>
+          <t>test.answer15</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>quest16</t>
+          <t>test.quest16</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
@@ -1342,12 +1346,12 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>quest65</t>
+          <t>test.quest65</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>answer66</t>
+          <t>test.answer66</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
@@ -1359,7 +1363,7 @@
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr">
         <is>
-          <t>['quest64']</t>
+          <t>['test.quest64']</t>
         </is>
       </c>
       <c r="I24" t="inlineStr"/>
@@ -1378,12 +1382,12 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>quest64</t>
+          <t>test.quest64</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>quest65</t>
+          <t>test.quest65</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
@@ -1395,7 +1399,7 @@
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr">
         <is>
-          <t>['answer63', 'answer58', 'answer39']</t>
+          <t>['test.answer63', 'test.answer58', 'test.answer39']</t>
         </is>
       </c>
       <c r="I25" t="inlineStr"/>
@@ -1416,12 +1420,12 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>answer63</t>
+          <t>test.answer63</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>quest64</t>
+          <t>test.quest64</t>
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
@@ -1433,7 +1437,7 @@
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr">
         <is>
-          <t>['quest62']</t>
+          <t>['test.quest62']</t>
         </is>
       </c>
       <c r="I26" t="inlineStr"/>
@@ -1454,12 +1458,12 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>answer58</t>
+          <t>test.answer58</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>quest64</t>
+          <t>test.quest64</t>
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
@@ -1471,7 +1475,7 @@
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr">
         <is>
-          <t>['quest57']</t>
+          <t>['test.quest57']</t>
         </is>
       </c>
       <c r="I27" t="inlineStr"/>
@@ -1492,12 +1496,12 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>answer39</t>
+          <t>test.answer39</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>quest64</t>
+          <t>test.quest64</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
@@ -1509,7 +1513,7 @@
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr">
         <is>
-          <t>['quest38']</t>
+          <t>['test.quest38']</t>
         </is>
       </c>
       <c r="I28" t="inlineStr"/>
@@ -1528,12 +1532,12 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>quest38</t>
+          <t>test.quest38</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>answer39</t>
+          <t>test.answer39</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
@@ -1545,7 +1549,7 @@
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr">
         <is>
-          <t>['quest37']</t>
+          <t>['test.quest37']</t>
         </is>
       </c>
       <c r="I29" t="inlineStr"/>
@@ -1564,12 +1568,12 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>quest37</t>
+          <t>test.quest37</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>quest38</t>
+          <t>test.quest38</t>
         </is>
       </c>
       <c r="E30" t="inlineStr"/>
@@ -1581,7 +1585,7 @@
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
-          <t>['quest36', 'answer35', 'answer33', 'answer31', 'answer25']</t>
+          <t>['test.quest36', 'test.answer35', 'test.answer33', 'test.answer31', 'test.answer25']</t>
         </is>
       </c>
       <c r="I30" t="inlineStr"/>
@@ -1607,12 +1611,12 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>quest36</t>
+          <t>test.quest36</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>quest37</t>
+          <t>test.quest37</t>
         </is>
       </c>
       <c r="E31" t="inlineStr"/>
@@ -1645,12 +1649,12 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>answer35</t>
+          <t>test.answer35</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>quest37</t>
+          <t>test.quest37</t>
         </is>
       </c>
       <c r="E32" t="inlineStr"/>
@@ -1662,7 +1666,7 @@
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr">
         <is>
-          <t>['quest34']</t>
+          <t>['test.quest34']</t>
         </is>
       </c>
       <c r="I32" t="inlineStr"/>
@@ -1683,12 +1687,12 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>answer33</t>
+          <t>test.answer33</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>quest37</t>
+          <t>test.quest37</t>
         </is>
       </c>
       <c r="E33" t="inlineStr"/>
@@ -1700,7 +1704,7 @@
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr">
         <is>
-          <t>['quest32']</t>
+          <t>['test.quest32']</t>
         </is>
       </c>
       <c r="I33" t="inlineStr"/>
@@ -1721,12 +1725,12 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>answer31</t>
+          <t>test.answer31</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>quest37</t>
+          <t>test.quest37</t>
         </is>
       </c>
       <c r="E34" t="inlineStr"/>
@@ -1738,7 +1742,7 @@
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr">
         <is>
-          <t>['quest30']</t>
+          <t>['test.quest30']</t>
         </is>
       </c>
       <c r="I34" t="inlineStr"/>
@@ -1759,12 +1763,12 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>answer25</t>
+          <t>test.answer25</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>quest37</t>
+          <t>test.quest37</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
@@ -1776,7 +1780,7 @@
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr">
         <is>
-          <t>['quest24']</t>
+          <t>['test.quest24']</t>
         </is>
       </c>
       <c r="I35" t="inlineStr"/>
@@ -1795,12 +1799,12 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>quest24</t>
+          <t>test.quest24</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>answer25</t>
+          <t>test.answer25</t>
         </is>
       </c>
       <c r="E36" t="inlineStr"/>
@@ -1812,7 +1816,7 @@
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
         <is>
-          <t>['answer23', 'answer21']</t>
+          <t>['test.answer23', 'test.answer21']</t>
         </is>
       </c>
       <c r="I36" t="inlineStr"/>
@@ -1832,12 +1836,12 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>answer23</t>
+          <t>test.answer23</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>quest24</t>
+          <t>test.quest24</t>
         </is>
       </c>
       <c r="E37" t="inlineStr"/>
@@ -1849,7 +1853,7 @@
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr">
         <is>
-          <t>['quest22']</t>
+          <t>['test.quest22']</t>
         </is>
       </c>
       <c r="I37" t="inlineStr"/>
@@ -1869,12 +1873,12 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>answer21</t>
+          <t>test.answer21</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>quest24</t>
+          <t>test.quest24</t>
         </is>
       </c>
       <c r="E38" t="inlineStr"/>
@@ -1886,7 +1890,7 @@
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr">
         <is>
-          <t>['quest20']</t>
+          <t>['test.quest20']</t>
         </is>
       </c>
       <c r="I38" t="inlineStr"/>
@@ -1907,12 +1911,12 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>quest20</t>
+          <t>test.quest20</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>answer21</t>
+          <t>test.answer21</t>
         </is>
       </c>
       <c r="E39" t="inlineStr"/>
@@ -1945,12 +1949,12 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>quest22</t>
+          <t>test.quest22</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>answer23</t>
+          <t>test.answer23</t>
         </is>
       </c>
       <c r="E40" t="inlineStr"/>
@@ -1981,12 +1985,12 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>quest30</t>
+          <t>test.quest30</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>answer31</t>
+          <t>test.answer31</t>
         </is>
       </c>
       <c r="E41" t="inlineStr"/>
@@ -1998,7 +2002,7 @@
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
-          <t>['answer29', 'answer27']</t>
+          <t>['test.answer29', 'test.answer27']</t>
         </is>
       </c>
       <c r="I41" t="inlineStr"/>
@@ -2026,12 +2030,12 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>answer29</t>
+          <t>test.answer29</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>quest30</t>
+          <t>test.quest30</t>
         </is>
       </c>
       <c r="E42" t="inlineStr"/>
@@ -2043,7 +2047,7 @@
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr">
         <is>
-          <t>['quest28']</t>
+          <t>['test.quest28']</t>
         </is>
       </c>
       <c r="I42" t="inlineStr"/>
@@ -2063,12 +2067,12 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>answer27</t>
+          <t>test.answer27</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>quest30</t>
+          <t>test.quest30</t>
         </is>
       </c>
       <c r="E43" t="inlineStr"/>
@@ -2080,7 +2084,7 @@
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
         <is>
-          <t>['quest26']</t>
+          <t>['test.quest26']</t>
         </is>
       </c>
       <c r="I43" t="inlineStr"/>
@@ -2101,12 +2105,12 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>quest26</t>
+          <t>test.quest26</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>answer27</t>
+          <t>test.answer27</t>
         </is>
       </c>
       <c r="E44" t="inlineStr"/>
@@ -2139,12 +2143,12 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>quest28</t>
+          <t>test.quest28</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>answer29</t>
+          <t>test.answer29</t>
         </is>
       </c>
       <c r="E45" t="inlineStr"/>
@@ -2188,12 +2192,12 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>quest32</t>
+          <t>test.quest32</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>answer33</t>
+          <t>test.answer33</t>
         </is>
       </c>
       <c r="E46" t="inlineStr"/>
@@ -2235,12 +2239,12 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>quest34</t>
+          <t>test.quest34</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>answer35</t>
+          <t>test.answer35</t>
         </is>
       </c>
       <c r="E47" t="inlineStr"/>
@@ -2272,12 +2276,12 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>quest57</t>
+          <t>test.quest57</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>answer58</t>
+          <t>test.answer58</t>
         </is>
       </c>
       <c r="E48" t="inlineStr"/>
@@ -2289,7 +2293,7 @@
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
         <is>
-          <t>['quest56']</t>
+          <t>['test.quest56']</t>
         </is>
       </c>
       <c r="I48" t="inlineStr"/>
@@ -2310,12 +2314,12 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>quest56</t>
+          <t>test.quest56</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>quest57</t>
+          <t>test.quest57</t>
         </is>
       </c>
       <c r="E49" t="inlineStr"/>
@@ -2327,7 +2331,7 @@
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
         <is>
-          <t>['quest55', 'answer54', 'answer43', 'answer41']</t>
+          <t>['test.quest55', 'test.answer54', 'test.answer43', 'test.answer41']</t>
         </is>
       </c>
       <c r="I49" t="inlineStr"/>
@@ -2353,12 +2357,12 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>quest55</t>
+          <t>test.quest55</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>quest56</t>
+          <t>test.quest56</t>
         </is>
       </c>
       <c r="E50" t="inlineStr"/>
@@ -2391,12 +2395,12 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>answer54</t>
+          <t>test.answer54</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>quest56</t>
+          <t>test.quest56</t>
         </is>
       </c>
       <c r="E51" t="inlineStr"/>
@@ -2408,7 +2412,7 @@
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr">
         <is>
-          <t>['quest53']</t>
+          <t>['test.quest53']</t>
         </is>
       </c>
       <c r="I51" t="inlineStr"/>
@@ -2428,12 +2432,12 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>answer43</t>
+          <t>test.answer43</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>quest56</t>
+          <t>test.quest56</t>
         </is>
       </c>
       <c r="E52" t="inlineStr"/>
@@ -2445,7 +2449,7 @@
       <c r="G52" t="inlineStr"/>
       <c r="H52" t="inlineStr">
         <is>
-          <t>['quest42']</t>
+          <t>['test.quest42']</t>
         </is>
       </c>
       <c r="I52" t="inlineStr"/>
@@ -2466,12 +2470,12 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>answer41</t>
+          <t>test.answer41</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>quest56</t>
+          <t>test.quest56</t>
         </is>
       </c>
       <c r="E53" t="inlineStr"/>
@@ -2483,7 +2487,7 @@
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr">
         <is>
-          <t>['quest40']</t>
+          <t>['test.quest40']</t>
         </is>
       </c>
       <c r="I53" t="inlineStr"/>
@@ -2509,12 +2513,12 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>quest40</t>
+          <t>test.quest40</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>answer41</t>
+          <t>test.answer41</t>
         </is>
       </c>
       <c r="E54" t="inlineStr"/>
@@ -2555,12 +2559,12 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>quest42</t>
+          <t>test.quest42</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>answer43</t>
+          <t>test.answer43</t>
         </is>
       </c>
       <c r="E55" t="inlineStr"/>
@@ -2591,12 +2595,12 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>quest53</t>
+          <t>test.quest53</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>answer54</t>
+          <t>test.answer54</t>
         </is>
       </c>
       <c r="E56" t="inlineStr"/>
@@ -2608,7 +2612,7 @@
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
         <is>
-          <t>['quest52']</t>
+          <t>['test.quest52']</t>
         </is>
       </c>
       <c r="I56" t="inlineStr"/>
@@ -2629,12 +2633,12 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>quest52</t>
+          <t>test.quest52</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>quest53</t>
+          <t>test.quest53</t>
         </is>
       </c>
       <c r="E57" t="inlineStr"/>
@@ -2646,7 +2650,7 @@
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr">
         <is>
-          <t>['answer51', 'answer49', 'answer47', 'answer45']</t>
+          <t>['test.answer51', 'test.answer49', 'test.answer47', 'test.answer45']</t>
         </is>
       </c>
       <c r="I57" t="inlineStr"/>
@@ -2667,12 +2671,12 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>answer51</t>
+          <t>test.answer51</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>quest52</t>
+          <t>test.quest52</t>
         </is>
       </c>
       <c r="E58" t="inlineStr"/>
@@ -2684,7 +2688,7 @@
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
         <is>
-          <t>['quest50']</t>
+          <t>['test.quest50']</t>
         </is>
       </c>
       <c r="I58" t="inlineStr"/>
@@ -2705,12 +2709,12 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>answer49</t>
+          <t>test.answer49</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>quest52</t>
+          <t>test.quest52</t>
         </is>
       </c>
       <c r="E59" t="inlineStr"/>
@@ -2722,7 +2726,7 @@
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr">
         <is>
-          <t>['quest48']</t>
+          <t>['test.quest48']</t>
         </is>
       </c>
       <c r="I59" t="inlineStr"/>
@@ -2743,12 +2747,12 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>answer47</t>
+          <t>test.answer47</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>quest52</t>
+          <t>test.quest52</t>
         </is>
       </c>
       <c r="E60" t="inlineStr"/>
@@ -2760,7 +2764,7 @@
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="inlineStr">
         <is>
-          <t>['quest46']</t>
+          <t>['test.quest46']</t>
         </is>
       </c>
       <c r="I60" t="inlineStr"/>
@@ -2781,12 +2785,12 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>answer45</t>
+          <t>test.answer45</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>quest52</t>
+          <t>test.quest52</t>
         </is>
       </c>
       <c r="E61" t="inlineStr"/>
@@ -2798,7 +2802,7 @@
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
         <is>
-          <t>['quest44']</t>
+          <t>['test.quest44']</t>
         </is>
       </c>
       <c r="I61" t="inlineStr"/>
@@ -2819,12 +2823,12 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>quest44</t>
+          <t>test.quest44</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>answer45</t>
+          <t>test.answer45</t>
         </is>
       </c>
       <c r="E62" t="inlineStr"/>
@@ -2857,12 +2861,12 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>quest46</t>
+          <t>test.quest46</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>answer47</t>
+          <t>test.answer47</t>
         </is>
       </c>
       <c r="E63" t="inlineStr"/>
@@ -2900,12 +2904,12 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>quest48</t>
+          <t>test.quest48</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>answer49</t>
+          <t>test.answer49</t>
         </is>
       </c>
       <c r="E64" t="inlineStr"/>
@@ -2938,12 +2942,12 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>quest50</t>
+          <t>test.quest50</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>answer51</t>
+          <t>test.answer51</t>
         </is>
       </c>
       <c r="E65" t="inlineStr"/>
@@ -2975,12 +2979,12 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>quest62</t>
+          <t>test.quest62</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>answer63</t>
+          <t>test.answer63</t>
         </is>
       </c>
       <c r="E66" t="inlineStr"/>
@@ -2992,7 +2996,7 @@
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
         <is>
-          <t>['answer61']</t>
+          <t>['test.answer61']</t>
         </is>
       </c>
       <c r="I66" t="inlineStr"/>
@@ -3012,12 +3016,12 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>answer61</t>
+          <t>test.answer61</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>quest62</t>
+          <t>test.quest62</t>
         </is>
       </c>
       <c r="E67" t="inlineStr"/>
@@ -3029,7 +3033,7 @@
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
         <is>
-          <t>['quest60']</t>
+          <t>['test.quest60']</t>
         </is>
       </c>
       <c r="I67" t="inlineStr"/>
@@ -3058,12 +3062,12 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>quest60</t>
+          <t>test.quest60</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>answer61</t>
+          <t>test.answer61</t>
         </is>
       </c>
       <c r="E68" t="inlineStr"/>
@@ -3075,7 +3079,7 @@
       <c r="G68" t="inlineStr"/>
       <c r="H68" t="inlineStr">
         <is>
-          <t>['answer59']</t>
+          <t>['test.answer59']</t>
         </is>
       </c>
       <c r="I68" t="inlineStr"/>
@@ -3093,12 +3097,12 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>answer59</t>
+          <t>test.answer59</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>quest60</t>
+          <t>test.quest60</t>
         </is>
       </c>
       <c r="E69" t="inlineStr"/>
@@ -3135,7 +3139,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>test.hero</t>
+          <t>test.test.hero</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -3191,7 +3195,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>test.npc</t>
+          <t>test.test.npc</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -3240,7 +3244,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>test.remarka</t>
+          <t>test.test.remarka</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">

</xml_diff>